<commit_message>
Add discount and T2 tax to excel template
</commit_message>
<xml_diff>
--- a/public/ExcelTemplates/InvoiceUpload.xlsx
+++ b/public/ExcelTemplates/InvoiceUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Desktop\HMO\Excel Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF5F399-9DE6-4D00-89AD-DABB0D9B2DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4230CABF-35B7-41F9-8FFD-CCB6EAEBC457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>internalID</t>
   </si>
@@ -106,16 +106,25 @@
     <t>ST</t>
   </si>
   <si>
-    <t>00100</t>
-  </si>
-  <si>
     <t>11/14/2021</t>
   </si>
   <si>
-    <t>EG-XXXX-ZZZ</t>
-  </si>
-  <si>
-    <t>0123</t>
+    <t>T2(Tbl01)</t>
+  </si>
+  <si>
+    <t>itemsDiscount</t>
+  </si>
+  <si>
+    <t>خصم الأصناف</t>
+  </si>
+  <si>
+    <t>EG-237791390-QTC1012</t>
+  </si>
+  <si>
+    <t>netTotal</t>
+  </si>
+  <si>
+    <t>الصافى (بعد الخصم قبل الضريبة)</t>
   </si>
 </sst>
 </file>
@@ -958,30 +967,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1016,16 +1027,25 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1060,39 +1080,48 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
+      <c r="Q2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>28</v>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>500</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4690</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -1101,16 +1130,25 @@
         <v>100</v>
       </c>
       <c r="K3">
+        <v>1100</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
         <v>1000</v>
       </c>
-      <c r="L3">
-        <v>1077</v>
-      </c>
-      <c r="M3">
-        <v>77</v>
-      </c>
       <c r="N3">
+        <v>1145</v>
+      </c>
+      <c r="O3">
+        <v>140</v>
+      </c>
+      <c r="P3">
         <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Credit/Debit to upload excel invoices
</commit_message>
<xml_diff>
--- a/public/ExcelTemplates/InvoiceUpload.xlsx
+++ b/public/ExcelTemplates/InvoiceUpload.xlsx
@@ -5,17 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoud.fayez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4230CABF-35B7-41F9-8FFD-CCB6EAEBC457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C3BF20-A15D-49CA-A092-885584F1A7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -64,9 +75,6 @@
     <t>T1(V001)</t>
   </si>
   <si>
-    <t>EGP</t>
-  </si>
-  <si>
     <t>رقم الفرع</t>
   </si>
   <si>
@@ -79,15 +87,9 @@
     <t>كود الصنف</t>
   </si>
   <si>
-    <t>وحدة القياس</t>
-  </si>
-  <si>
     <t>الكمية</t>
   </si>
   <si>
-    <t>العملة</t>
-  </si>
-  <si>
     <t>أجمالى السعر</t>
   </si>
   <si>
@@ -100,15 +102,6 @@
     <t>رقم الفاتورة</t>
   </si>
   <si>
-    <t>رقم المشترى</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
-    <t>11/14/2021</t>
-  </si>
-  <si>
     <t>T2(Tbl01)</t>
   </si>
   <si>
@@ -118,13 +111,39 @@
     <t>خصم الأصناف</t>
   </si>
   <si>
-    <t>EG-237791390-QTC1012</t>
-  </si>
-  <si>
     <t>netTotal</t>
   </si>
   <si>
     <t>الصافى (بعد الخصم قبل الضريبة)</t>
+  </si>
+  <si>
+    <t>documentType</t>
+  </si>
+  <si>
+    <t>فاتورة: I
+مرتجع: C
+اضافة: D</t>
+  </si>
+  <si>
+    <t>مرتجع</t>
+  </si>
+  <si>
+    <t>رقم المشترى
+الرقم المسلسل فى البرنامج</t>
+  </si>
+  <si>
+    <t>11/30/2022</t>
+  </si>
+  <si>
+    <t>وحدة القياس
+قطعة:EA
+كارتونة:CT
+كيلوجرام:KGM
+شرنك:SH
+لتر:LTR</t>
+  </si>
+  <si>
+    <t>العملة (EGP)</t>
   </si>
 </sst>
 </file>
@@ -608,10 +627,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -967,191 +996,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
-        <v>29</v>
+      <c r="R2" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>500</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4690</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3">
-        <v>1100</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3">
-        <v>1000</v>
-      </c>
-      <c r="N3">
-        <v>1145</v>
-      </c>
-      <c r="O3">
-        <v>140</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>5</v>
-      </c>
+      <c r="F3" s="1">
+        <v>4630</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{047A064C-A425-431A-9126-1A0FECFD1F87}">
+      <formula1>"فاتورة,مرتجع,أضافة,I,C,D"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{A1853929-3725-435C-B63C-A2082D5B1237}">
+      <formula1>"EA,CT,KGM,SH,LTR"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>